<commit_message>
Added interview with David Blazar, modded Excel file.
Open on any computer.
</commit_message>
<xml_diff>
--- a/School Budgets Project/Schools Spending, Diversity Isolated.xlsx
+++ b/School Budgets Project/Schools Spending, Diversity Isolated.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/halas/Documents/GitHub/CNS-Digital-Materials/School Budgets Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\helio\OneDrive\Documents\GitHub\CNS Digital Materials\School Budgets Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A01E260-F861-064D-BCAC-6EA910D130F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{4A01E260-F861-064D-BCAC-6EA910D130F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{82E20565-F35F-4BD5-AA23-7B956E51B53D}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="2360" windowWidth="27640" windowHeight="16940" xr2:uid="{6C415746-AC02-AC48-BC56-32A50562C304}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{6C415746-AC02-AC48-BC56-32A50562C304}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$26</definedName>
+  </definedNames>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -540,17 +544,17 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
     <col min="4" max="4" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="71">
+    <row r="1" spans="1:4" ht="66.400000000000006">
       <c r="A1" s="8" t="s">
         <v>25</v>
       </c>
@@ -590,7 +594,7 @@
         <v>53.9</v>
       </c>
       <c r="D3" s="9">
-        <f t="shared" ref="D3:D26" si="0">RANK(C3, $C$2:$C$25, 1)</f>
+        <f>RANK(C3, $C$2:$C$25, 1)</f>
         <v>10</v>
       </c>
     </row>
@@ -605,7 +609,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="9">
-        <f t="shared" si="0"/>
+        <f>RANK(C4, $C$2:$C$25, 1)</f>
         <v>2</v>
       </c>
     </row>
@@ -620,7 +624,7 @@
         <v>38.700000000000003</v>
       </c>
       <c r="D5" s="9">
-        <f t="shared" si="0"/>
+        <f>RANK(C5, $C$2:$C$25, 1)</f>
         <v>6</v>
       </c>
     </row>
@@ -635,7 +639,7 @@
         <v>71.2</v>
       </c>
       <c r="D6" s="9">
-        <f t="shared" si="0"/>
+        <f>RANK(C6, $C$2:$C$25, 1)</f>
         <v>19</v>
       </c>
     </row>
@@ -650,7 +654,7 @@
         <v>62.7</v>
       </c>
       <c r="D7" s="9">
-        <f t="shared" si="0"/>
+        <f>RANK(C7, $C$2:$C$25, 1)</f>
         <v>14</v>
       </c>
     </row>
@@ -665,7 +669,7 @@
         <v>83.5</v>
       </c>
       <c r="D8" s="9">
-        <f t="shared" si="0"/>
+        <f>RANK(C8, $C$2:$C$25, 1)</f>
         <v>22</v>
       </c>
     </row>
@@ -680,7 +684,7 @@
         <v>76.8</v>
       </c>
       <c r="D9" s="9">
-        <f t="shared" si="0"/>
+        <f>RANK(C9, $C$2:$C$25, 1)</f>
         <v>20</v>
       </c>
     </row>
@@ -695,7 +699,7 @@
         <v>25.2</v>
       </c>
       <c r="D10" s="9">
-        <f t="shared" si="0"/>
+        <f>RANK(C10, $C$2:$C$25, 1)</f>
         <v>3</v>
       </c>
     </row>
@@ -710,7 +714,7 @@
         <v>43.2</v>
       </c>
       <c r="D11" s="9">
-        <f t="shared" si="0"/>
+        <f>RANK(C11, $C$2:$C$25, 1)</f>
         <v>9</v>
       </c>
     </row>
@@ -725,7 +729,7 @@
         <v>60.4</v>
       </c>
       <c r="D12" s="9">
-        <f t="shared" si="0"/>
+        <f>RANK(C12, $C$2:$C$25, 1)</f>
         <v>12</v>
       </c>
     </row>
@@ -740,7 +744,7 @@
         <v>96.4</v>
       </c>
       <c r="D13" s="9">
-        <f t="shared" si="0"/>
+        <f>RANK(C13, $C$2:$C$25, 1)</f>
         <v>24</v>
       </c>
     </row>
@@ -755,7 +759,7 @@
         <v>63.7</v>
       </c>
       <c r="D14" s="9">
-        <f t="shared" si="0"/>
+        <f>RANK(C14, $C$2:$C$25, 1)</f>
         <v>15</v>
       </c>
     </row>
@@ -770,7 +774,7 @@
         <v>37.299999999999997</v>
       </c>
       <c r="D15" s="9">
-        <f t="shared" si="0"/>
+        <f>RANK(C15, $C$2:$C$25, 1)</f>
         <v>5</v>
       </c>
     </row>
@@ -785,7 +789,7 @@
         <v>60.9</v>
       </c>
       <c r="D16" s="9">
-        <f t="shared" si="0"/>
+        <f>RANK(C16, $C$2:$C$25, 1)</f>
         <v>13</v>
       </c>
     </row>
@@ -800,7 +804,7 @@
         <v>28.3</v>
       </c>
       <c r="D17" s="9">
-        <f t="shared" si="0"/>
+        <f>RANK(C17, $C$2:$C$25, 1)</f>
         <v>4</v>
       </c>
     </row>
@@ -815,7 +819,7 @@
         <v>4.2</v>
       </c>
       <c r="D18" s="9">
-        <f t="shared" si="0"/>
+        <f>RANK(C18, $C$2:$C$25, 1)</f>
         <v>1</v>
       </c>
     </row>
@@ -830,7 +834,7 @@
         <v>79.599999999999994</v>
       </c>
       <c r="D19" s="9">
-        <f t="shared" si="0"/>
+        <f>RANK(C19, $C$2:$C$25, 1)</f>
         <v>21</v>
       </c>
     </row>
@@ -845,7 +849,7 @@
         <v>64.099999999999994</v>
       </c>
       <c r="D20" s="9">
-        <f t="shared" si="0"/>
+        <f>RANK(C20, $C$2:$C$25, 1)</f>
         <v>16</v>
       </c>
     </row>
@@ -860,7 +864,7 @@
         <v>39</v>
       </c>
       <c r="D21" s="9">
-        <f t="shared" si="0"/>
+        <f>RANK(C21, $C$2:$C$25, 1)</f>
         <v>7</v>
       </c>
     </row>
@@ -875,7 +879,7 @@
         <v>58.4</v>
       </c>
       <c r="D22" s="9">
-        <f t="shared" si="0"/>
+        <f>RANK(C22, $C$2:$C$25, 1)</f>
         <v>11</v>
       </c>
     </row>
@@ -890,7 +894,7 @@
         <v>67.2</v>
       </c>
       <c r="D23" s="9">
-        <f t="shared" si="0"/>
+        <f>RANK(C23, $C$2:$C$25, 1)</f>
         <v>18</v>
       </c>
     </row>
@@ -905,7 +909,7 @@
         <v>42.6</v>
       </c>
       <c r="D24" s="9">
-        <f t="shared" si="0"/>
+        <f>RANK(C24, $C$2:$C$25, 1)</f>
         <v>8</v>
       </c>
     </row>
@@ -920,7 +924,7 @@
         <v>65.400000000000006</v>
       </c>
       <c r="D25" s="9">
-        <f t="shared" si="0"/>
+        <f>RANK(C25, $C$2:$C$25, 1)</f>
         <v>17</v>
       </c>
     </row>
@@ -935,7 +939,7 @@
         <v>37.299999999999997</v>
       </c>
       <c r="D26" s="9">
-        <f t="shared" si="0"/>
+        <f>RANK(C26, $C$2:$C$25, 1)</f>
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Eh, I'm not really sure lol.
</commit_message>
<xml_diff>
--- a/School Budgets Project/Schools Spending, Diversity Isolated.xlsx
+++ b/School Budgets Project/Schools Spending, Diversity Isolated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\helio\OneDrive\Documents\GitHub\CNS Digital Materials\School Budgets Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{4A01E260-F861-064D-BCAC-6EA910D130F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BDBC494C-1493-496B-85B0-0D660F51924C}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{4A01E260-F861-064D-BCAC-6EA910D130F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{55C92892-FE91-498F-BDB6-DFA6F6864698}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{6C415746-AC02-AC48-BC56-32A50562C304}"/>
   </bookViews>
@@ -548,7 +548,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -581,7 +581,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3">
-        <v>18558.299802989917</v>
+        <v>3770</v>
       </c>
       <c r="C2" s="5">
         <v>88</v>
@@ -591,8 +591,8 @@
         <v>23</v>
       </c>
       <c r="E2" s="10">
-        <f>RANK(B2, $B$2:$B$26, 0)</f>
-        <v>5</v>
+        <f>RANK(B2, $B$2:$B$25, 0)</f>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -600,7 +600,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3">
-        <v>17261.467678219797</v>
+        <v>8482</v>
       </c>
       <c r="C3" s="5">
         <v>53.9</v>
@@ -610,8 +610,8 @@
         <v>10</v>
       </c>
       <c r="E3" s="10">
-        <f t="shared" ref="E3:E26" si="1">RANK(B3, $B$2:$B$26, 0)</f>
-        <v>12</v>
+        <f t="shared" ref="E3:E25" si="1">RANK(B3, $B$2:$B$25, 0)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -619,7 +619,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>19062.04</v>
+        <v>3703</v>
       </c>
       <c r="C4" s="5">
         <v>8</v>
@@ -630,7 +630,7 @@
       </c>
       <c r="E4" s="10">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -638,7 +638,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="4">
-        <v>17391.706440564256</v>
+        <v>7426</v>
       </c>
       <c r="C5" s="5">
         <v>38.700000000000003</v>
@@ -657,7 +657,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4">
-        <v>17153.368493839578</v>
+        <v>8153</v>
       </c>
       <c r="C6" s="5">
         <v>71.2</v>
@@ -668,7 +668,7 @@
       </c>
       <c r="E6" s="10">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -676,7 +676,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="4">
-        <v>15030.828754104026</v>
+        <v>2617</v>
       </c>
       <c r="C7" s="5">
         <v>62.7</v>
@@ -687,7 +687,7 @@
       </c>
       <c r="E7" s="10">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -695,7 +695,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="4">
-        <v>15101.461447212338</v>
+        <v>7749</v>
       </c>
       <c r="C8" s="5">
         <v>83.5</v>
@@ -706,7 +706,7 @@
       </c>
       <c r="E8" s="10">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -714,7 +714,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="4">
-        <v>15761.42970580578</v>
+        <v>5616</v>
       </c>
       <c r="C9" s="5">
         <v>76.8</v>
@@ -725,7 +725,7 @@
       </c>
       <c r="E9" s="10">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -733,7 +733,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="4">
-        <v>16944.221747052918</v>
+        <v>6921</v>
       </c>
       <c r="C10" s="5">
         <v>25.2</v>
@@ -744,7 +744,7 @@
       </c>
       <c r="E10" s="10">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -752,7 +752,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="4">
-        <v>20293.352003356409</v>
+        <v>4232</v>
       </c>
       <c r="C11" s="5">
         <v>43.2</v>
@@ -763,7 +763,7 @@
       </c>
       <c r="E11" s="10">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -771,7 +771,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="4">
-        <v>17238.23597532036</v>
+        <v>6571</v>
       </c>
       <c r="C12" s="5">
         <v>60.4</v>
@@ -782,7 +782,7 @@
       </c>
       <c r="E12" s="10">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -790,7 +790,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="4">
-        <v>15547.735240094464</v>
+        <v>7496</v>
       </c>
       <c r="C13" s="5">
         <v>96.4</v>
@@ -801,7 +801,7 @@
       </c>
       <c r="E13" s="10">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -809,7 +809,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="4">
-        <v>15435.736103758602</v>
+        <v>6666</v>
       </c>
       <c r="C14" s="5">
         <v>63.7</v>
@@ -820,7 +820,7 @@
       </c>
       <c r="E14" s="10">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -828,7 +828,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="4">
-        <v>18016.971787827559</v>
+        <v>10603</v>
       </c>
       <c r="C15" s="5">
         <v>37.299999999999997</v>
@@ -839,7 +839,7 @@
       </c>
       <c r="E15" s="10">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -847,7 +847,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="4">
-        <v>15721.459106874059</v>
+        <v>9572</v>
       </c>
       <c r="C16" s="5">
         <v>60.9</v>
@@ -858,7 +858,7 @@
       </c>
       <c r="E16" s="10">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -866,7 +866,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="4">
-        <v>21311.797717058918</v>
+        <v>10807</v>
       </c>
       <c r="C17" s="5">
         <v>28.3</v>
@@ -876,8 +876,8 @@
         <v>4</v>
       </c>
       <c r="E17" s="10">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <f>E19</f>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -885,7 +885,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="4">
-        <v>17881.637369447257</v>
+        <v>5982</v>
       </c>
       <c r="C18" s="5">
         <v>4.2</v>
@@ -896,7 +896,7 @@
       </c>
       <c r="E18" s="10">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -904,7 +904,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="4">
-        <v>14214.016070969401</v>
+        <v>7584</v>
       </c>
       <c r="C19" s="5">
         <v>79.599999999999994</v>
@@ -915,7 +915,7 @@
       </c>
       <c r="E19" s="10">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -923,7 +923,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="4">
-        <v>14299.929153049354</v>
+        <v>6092</v>
       </c>
       <c r="C20" s="5">
         <v>64.099999999999994</v>
@@ -934,7 +934,7 @@
       </c>
       <c r="E20" s="10">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -942,7 +942,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="4">
-        <v>21330.260109664152</v>
+        <v>3618</v>
       </c>
       <c r="C21" s="5">
         <v>39</v>
@@ -953,7 +953,7 @@
       </c>
       <c r="E21" s="10">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -961,7 +961,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="4">
-        <v>14387.828454584589</v>
+        <v>9251</v>
       </c>
       <c r="C22" s="5">
         <v>58.4</v>
@@ -972,7 +972,7 @@
       </c>
       <c r="E22" s="10">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -980,7 +980,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="4">
-        <v>14589.274574020801</v>
+        <v>4518</v>
       </c>
       <c r="C23" s="5">
         <v>67.2</v>
@@ -991,7 +991,7 @@
       </c>
       <c r="E23" s="10">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -999,7 +999,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="4">
-        <v>17704.902494482714</v>
+        <v>2963</v>
       </c>
       <c r="C24" s="5">
         <v>42.6</v>
@@ -1010,7 +1010,7 @@
       </c>
       <c r="E24" s="10">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1018,7 +1018,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="4">
-        <v>18507.128366247754</v>
+        <v>13528</v>
       </c>
       <c r="C25" s="5">
         <v>65.400000000000006</v>
@@ -1029,27 +1029,19 @@
       </c>
       <c r="E25" s="10">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="4">
-        <v>17992.621208272678</v>
-      </c>
+      <c r="B26" s="4"/>
       <c r="C26" s="5">
         <v>37.299999999999997</v>
       </c>
-      <c r="D26" s="9">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E26" s="10">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>